<commit_message>
edit and add forms modyfications
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>fl_id</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>sql table</t>
-  </si>
-  <si>
-    <t>walidacja przy save w addForm czy PLU ma 6 cyfr</t>
   </si>
 </sst>
 </file>
@@ -182,6 +179,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066799" y="323850"/>
+          <a:ext cx="10772775" cy="6267450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> walidacja przy save w addForm czy PLU ma 6 cyfr</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t>- error jak klikasz np. na fairtrade w widoku kiwatów</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,20 +774,16 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="183.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
+    <row r="2" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export to excel from Avvik
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="todo" sheetId="2" r:id="rId3"/>
+    <sheet name="output" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
   <si>
     <t>fl_id</t>
   </si>
@@ -171,6 +171,144 @@
   </si>
   <si>
     <t>Deletes all selected lines or the current line if no selection has been made</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>PLU</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Stickers Text</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Bucket size</t>
+  </si>
+  <si>
+    <t>Sleeve's type</t>
+  </si>
+  <si>
+    <t>Production Sleeve</t>
+  </si>
+  <si>
+    <t>FOB</t>
+  </si>
+  <si>
+    <t>Price PrBunch</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>print stickers?</t>
+  </si>
+  <si>
+    <t>bunch PrBox</t>
+  </si>
+  <si>
+    <t>PrBucket</t>
+  </si>
+  <si>
+    <t>PrBunch</t>
+  </si>
+  <si>
+    <t>Pack rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boxes </t>
+  </si>
+  <si>
+    <t>buckets</t>
+  </si>
+  <si>
+    <t>stems</t>
+  </si>
+  <si>
+    <t>avvik</t>
+  </si>
+  <si>
+    <t>boxes</t>
+  </si>
+  <si>
+    <t>farms</t>
+  </si>
+  <si>
+    <t>Datecode</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>order - butikkdata</t>
+  </si>
+  <si>
+    <t>order number</t>
+  </si>
+  <si>
+    <t>departure</t>
+  </si>
+  <si>
+    <t>arrival</t>
+  </si>
+  <si>
+    <t>datecode</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>bokser</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>Sleeve</t>
+  </si>
+  <si>
+    <t>with sleeve</t>
+  </si>
+  <si>
+    <t>bunch pr bucket</t>
+  </si>
+  <si>
+    <t>stems pr bunch</t>
+  </si>
+  <si>
+    <t>bucket</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>pak rate</t>
+  </si>
+  <si>
+    <t>sleeve</t>
+  </si>
+  <si>
+    <t>ordre nummer</t>
   </si>
 </sst>
 </file>
@@ -208,7 +346,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +356,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -263,6 +431,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -977,4 +1151,432 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>